<commit_message>
Update latest lessons file
</commit_message>
<xml_diff>
--- a/lessons.xlsx
+++ b/lessons.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naval\Desktop\Data\MR ALGO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naval\Desktop\Data\DNT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDD17B66-5191-4065-B41F-5C7A215040A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59869432-97C7-48AF-B43E-BB840F768539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="perfect can u generate for 3 mo" sheetId="1" r:id="rId1"/>
+    <sheet name="Lessons" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -4099,7 +4099,7 @@
   <dimension ref="A1:E412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G168" sqref="G168:G169"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change time to 10:10 AM
</commit_message>
<xml_diff>
--- a/lessons.xlsx
+++ b/lessons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naval\Desktop\Data\DNT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daily-hindi-telegram-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59869432-97C7-48AF-B43E-BB840F768539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EC06A7-E02B-4576-A03C-C0CF7582E2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4099,7 +4099,7 @@
   <dimension ref="A1:E412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>